<commit_message>
modify before tree (#3)
</commit_message>
<xml_diff>
--- a/data/contig_annotation.xlsx
+++ b/data/contig_annotation.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allen/github/rujinlong/p0062/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allen/github/rujinlong/phydgene/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C5C718-D153-B34D-A135-C1A78EBB234A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BF1106-6FD5-1B49-B240-41F5698126E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{3130BB6A-7A0D-2D4D-BA4E-4B0EB43F77EA}"/>
+    <workbookView xWindow="34020" yWindow="-7080" windowWidth="51200" windowHeight="27480" activeTab="1" xr2:uid="{3130BB6A-7A0D-2D4D-BA4E-4B0EB43F77EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -6248,9 +6249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E327E45-D2E5-984F-9539-46C3E8BF068C}">
   <dimension ref="A1:E930"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -22079,8 +22078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5279EA80-AE4B-A04E-BA74-B4A8705C4E99}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22333,4 +22332,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA2E145-3B6C-8047-971F-8AB14D59682C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>